<commit_message>
Premier dépot non terminé
</commit_message>
<xml_diff>
--- a/base_de_donnees.xlsx
+++ b/base_de_donnees.xlsx
@@ -510,7 +510,7 @@
         <v>789922528</v>
       </c>
       <c r="F3" t="n">
-        <v>600000000</v>
+        <v>525000000</v>
       </c>
     </row>
     <row r="4">
@@ -534,7 +534,7 @@
         <v>748150337</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>25000000</v>
       </c>
     </row>
     <row r="5">
@@ -558,57 +558,55 @@
         <v>759909647</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>50000000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>19755</v>
+        <v>95585</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KOIKIWA</t>
+          <t>ZEGA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>KIKI</t>
+          <t>MARGUERITE LOUIS</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E6" t="n">
-        <v>303917676</v>
+        <v>102030405</v>
       </c>
       <c r="F6" t="n">
-        <v>50000</v>
+        <v>70000000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>39254</v>
+        <v>64258</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZEGA</t>
+          <t xml:space="preserve">KOUDOU </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LALA</t>
+          <t>LAURENT</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>12</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0747919391</t>
-        </is>
+        <v>73</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1234569</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>